<commit_message>
Excel Sheet Downloading Functionality Done
</commit_message>
<xml_diff>
--- a/sample_book.xlsx
+++ b/sample_book.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Changed Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Students Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,8 +48,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,8 +427,162 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
+          <t>Fullname</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Rollno</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Mobileno</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Riya Ingale</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>19102B0030</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>8692931133</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>riya.ingale@vit.edu.in</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CMPN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Swabhav Techlabs</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Python Programming</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Dhwani</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" s="1" t="n">
+        <v>44222</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>44252</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Samiksha</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>19102B0021</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>9892805720</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>samiksha143018@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>CMPN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Swabhav Techlabs</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Python Programming</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Dhwani</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" s="1" t="n">
+        <v>44222</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>44252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Internship Page Updated
</commit_message>
<xml_diff>
--- a/sample_book.xlsx
+++ b/sample_book.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -48,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -416,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +437,91 @@
           <t>Mobileno</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Division</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Domain</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>skills_required</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Company Representative Name</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Company Representative Contact</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>End Date</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Feedback</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Work Environment Rating</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Satisfaction</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Would student recommend?</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -484,17 +566,19 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Python Programming</t>
+          <t>Python Intern</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
+          <t>Web Development</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
           <t>Self</t>
         </is>
       </c>
-      <c r="K2" t="n">
-        <v>5</v>
-      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>Python</t>
@@ -506,83 +590,33 @@
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" s="1" t="n">
-        <v>44222</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>44252</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Samiksha</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>19102B0021</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>9892805720</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>samiksha143018@gmail.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>CMPN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>TE</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Swabhav Techlabs</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Python Programming</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Self</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>5</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Python</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Dhwani</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" s="1" t="n">
-        <v>44222</v>
-      </c>
-      <c r="P3" s="1" t="n">
-        <v>44252</v>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>22 /02 /21</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>21/ 03/ 21</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Nice Experience</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
+        <v>4</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Maybe</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new internship changes added
</commit_message>
<xml_diff>
--- a/sample_book.xlsx
+++ b/sample_book.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -715,6 +715,102 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Deep</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>19102B0052</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>09323165165</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>esotericdeep@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CMPN</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Swabhav Techlabs</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Python Intern</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Web Development</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Dhwani</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>22 /02 /21</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>21/ 03/ 21</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Nice Experience</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
+        <v>4</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Maybe</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Hyperlinks in Excel
</commit_message>
<xml_diff>
--- a/sample_book.xlsx
+++ b/sample_book.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,6 +522,11 @@
           <t>Would student recommend?</t>
         </is>
       </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Completition Certificate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -541,7 +546,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>riya.ingale@vit.edu.in</t>
+          <t>riya.ingale14@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -592,12 +597,12 @@
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>22 /02 /21</t>
+          <t>20 /01 /21</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>21/ 03/ 21</t>
+          <t>22/ 02/ 21</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -615,200 +620,12 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Maybe</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Samiksha Pansare</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>19102B0021</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>9892805720</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>samiksha143018@gmail.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>CMPN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>TE</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Swabhav Techlabs</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Python Intern</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Web Development</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Self</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Python</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Dhwani</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>22 /02 /21</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>21/ 03/ 21</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Nice Experience</t>
-        </is>
-      </c>
-      <c r="R3" t="n">
-        <v>4</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Maybe</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Deep</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>19102B0052</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>09323165165</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>esotericdeep@gmail.com</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>CMPN</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>TE</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Swabhav Techlabs</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Python Intern</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Web Development</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Self</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Python</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Dhwani</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>22 /02 /21</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>21/ 03/ 21</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Nice Experience</t>
-        </is>
-      </c>
-      <c r="R4" t="n">
-        <v>4</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Maybe</t>
-        </is>
+      <c r="U2">
+        <f>HYPERLINK("http://127.0.0.1:5000/downloadcompletioncert/1", "Download Cert")</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>